<commit_message>
create qcow2 image file
</commit_message>
<xml_diff>
--- a/001.vbr/layout/vbr_BPB_FAT12_16.xlsx
+++ b/001.vbr/layout/vbr_BPB_FAT12_16.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="153">
   <si>
     <t>サブシステム</t>
   </si>
@@ -1992,6 +1992,12 @@
   <si>
     <t>X(448)</t>
     <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>bs_Code</t>
+  </si>
+  <si>
+    <t>bs_EndFlag</t>
   </si>
 </sst>
 </file>
@@ -2965,46 +2971,10 @@
     <xf numFmtId="0" fontId="19" fillId="3" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="3" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3013,22 +2983,13 @@
     <xf numFmtId="0" fontId="23" fillId="3" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="3" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="3" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3043,7 +3004,19 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="3" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3056,6 +3029,18 @@
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="3" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3081,6 +3066,27 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
@@ -3513,9 +3519,9 @@
   <dimension ref="A1:Y26"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozenSplit"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="D10" sqref="D10"/>
-      <selection pane="bottomLeft" activeCell="AD15" sqref="AD15"/>
+      <selection pane="bottomLeft" activeCell="AB14" sqref="AB14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -5183,7 +5189,9 @@
       <c r="J25" s="88" t="s">
         <v>95</v>
       </c>
-      <c r="K25" s="88"/>
+      <c r="K25" s="88" t="s">
+        <v>151</v>
+      </c>
       <c r="L25" s="87"/>
       <c r="M25" s="87" t="s">
         <v>116</v>
@@ -5216,7 +5224,9 @@
       <c r="J26" s="88" t="s">
         <v>92</v>
       </c>
-      <c r="K26" s="88"/>
+      <c r="K26" s="88" t="s">
+        <v>152</v>
+      </c>
       <c r="L26" s="87"/>
       <c r="M26" s="87" t="s">
         <v>22</v>
@@ -5897,12 +5907,12 @@
   <sheetData>
     <row r="1" spans="1:59" ht="12.6" customHeight="1">
       <c r="C1" s="49"/>
-      <c r="D1" s="156" t="s">
+      <c r="D1" s="149" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="157"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="142" t="s">
+      <c r="E1" s="150"/>
+      <c r="F1" s="142"/>
+      <c r="G1" s="132" t="s">
         <v>31</v>
       </c>
       <c r="H1" s="120"/>
@@ -5911,80 +5921,80 @@
       <c r="K1" s="120"/>
       <c r="L1" s="120"/>
       <c r="M1" s="120"/>
-      <c r="N1" s="121"/>
-      <c r="O1" s="152" t="s">
+      <c r="N1" s="133"/>
+      <c r="O1" s="145" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="153"/>
+      <c r="P1" s="146"/>
       <c r="Q1" s="160" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="125" t="s">
+      <c r="R1" s="141" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="126"/>
-      <c r="T1" s="145" t="s">
+      <c r="S1" s="142"/>
+      <c r="T1" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="148" t="s">
+      <c r="U1" s="137" t="s">
         <v>33</v>
       </c>
-      <c r="V1" s="149"/>
-      <c r="W1" s="125" t="s">
+      <c r="V1" s="138"/>
+      <c r="W1" s="141" t="s">
         <v>34</v>
       </c>
-      <c r="X1" s="126"/>
-      <c r="Y1" s="145" t="s">
+      <c r="X1" s="142"/>
+      <c r="Y1" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="Z1" s="148" t="s">
+      <c r="Z1" s="137" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="149"/>
-      <c r="AB1" s="152" t="s">
+      <c r="AA1" s="138"/>
+      <c r="AB1" s="145" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="153"/>
-      <c r="AD1" s="125" t="s">
+      <c r="AC1" s="146"/>
+      <c r="AD1" s="141" t="s">
         <v>36</v>
       </c>
-      <c r="AE1" s="126"/>
-      <c r="AF1" s="140" t="s">
+      <c r="AE1" s="142"/>
+      <c r="AF1" s="122" t="s">
         <v>37</v>
       </c>
-      <c r="AG1" s="135"/>
-      <c r="AH1" s="135"/>
-      <c r="AI1" s="136"/>
-      <c r="AJ1" s="140" t="s">
+      <c r="AG1" s="123"/>
+      <c r="AH1" s="123"/>
+      <c r="AI1" s="124"/>
+      <c r="AJ1" s="122" t="s">
         <v>38</v>
       </c>
-      <c r="AK1" s="135"/>
-      <c r="AL1" s="135"/>
-      <c r="AM1" s="136"/>
-      <c r="AN1" s="143" t="s">
+      <c r="AK1" s="123"/>
+      <c r="AL1" s="123"/>
+      <c r="AM1" s="124"/>
+      <c r="AN1" s="128" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="143" t="s">
+      <c r="AO1" s="128" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" s="145" t="s">
+      <c r="AP1" s="130" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" s="142" t="s">
+      <c r="AQ1" s="132" t="s">
         <v>28</v>
       </c>
       <c r="AR1" s="120"/>
       <c r="AS1" s="120"/>
-      <c r="AT1" s="121"/>
-      <c r="AU1" s="131" t="s">
+      <c r="AT1" s="133"/>
+      <c r="AU1" s="153" t="s">
         <v>41</v>
       </c>
-      <c r="AV1" s="132"/>
-      <c r="AW1" s="132"/>
-      <c r="AX1" s="132"/>
-      <c r="AY1" s="132"/>
-      <c r="AZ1" s="132"/>
-      <c r="BA1" s="133"/>
+      <c r="AV1" s="154"/>
+      <c r="AW1" s="154"/>
+      <c r="AX1" s="154"/>
+      <c r="AY1" s="154"/>
+      <c r="AZ1" s="154"/>
+      <c r="BA1" s="155"/>
       <c r="BC1" s="50" t="s">
         <v>3</v>
       </c>
@@ -5997,56 +6007,56 @@
       <c r="C2" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="156"/>
-      <c r="E2" s="157"/>
-      <c r="F2" s="126"/>
-      <c r="G2" s="142"/>
+      <c r="D2" s="149"/>
+      <c r="E2" s="150"/>
+      <c r="F2" s="142"/>
+      <c r="G2" s="132"/>
       <c r="H2" s="120"/>
       <c r="I2" s="120"/>
       <c r="J2" s="120"/>
       <c r="K2" s="120"/>
       <c r="L2" s="120"/>
       <c r="M2" s="120"/>
-      <c r="N2" s="121"/>
-      <c r="O2" s="152"/>
-      <c r="P2" s="153"/>
+      <c r="N2" s="133"/>
+      <c r="O2" s="145"/>
+      <c r="P2" s="146"/>
       <c r="Q2" s="160"/>
-      <c r="R2" s="125"/>
-      <c r="S2" s="126"/>
-      <c r="T2" s="145"/>
-      <c r="U2" s="148"/>
-      <c r="V2" s="149"/>
-      <c r="W2" s="125"/>
-      <c r="X2" s="126"/>
-      <c r="Y2" s="145"/>
-      <c r="Z2" s="148"/>
-      <c r="AA2" s="149"/>
-      <c r="AB2" s="152"/>
-      <c r="AC2" s="153"/>
-      <c r="AD2" s="125"/>
-      <c r="AE2" s="126"/>
-      <c r="AF2" s="140"/>
-      <c r="AG2" s="135"/>
-      <c r="AH2" s="135"/>
-      <c r="AI2" s="136"/>
-      <c r="AJ2" s="140"/>
-      <c r="AK2" s="135"/>
-      <c r="AL2" s="135"/>
-      <c r="AM2" s="136"/>
-      <c r="AN2" s="143"/>
-      <c r="AO2" s="143"/>
-      <c r="AP2" s="145"/>
-      <c r="AQ2" s="142"/>
+      <c r="R2" s="141"/>
+      <c r="S2" s="142"/>
+      <c r="T2" s="130"/>
+      <c r="U2" s="137"/>
+      <c r="V2" s="138"/>
+      <c r="W2" s="141"/>
+      <c r="X2" s="142"/>
+      <c r="Y2" s="130"/>
+      <c r="Z2" s="137"/>
+      <c r="AA2" s="138"/>
+      <c r="AB2" s="145"/>
+      <c r="AC2" s="146"/>
+      <c r="AD2" s="141"/>
+      <c r="AE2" s="142"/>
+      <c r="AF2" s="122"/>
+      <c r="AG2" s="123"/>
+      <c r="AH2" s="123"/>
+      <c r="AI2" s="124"/>
+      <c r="AJ2" s="122"/>
+      <c r="AK2" s="123"/>
+      <c r="AL2" s="123"/>
+      <c r="AM2" s="124"/>
+      <c r="AN2" s="128"/>
+      <c r="AO2" s="128"/>
+      <c r="AP2" s="130"/>
+      <c r="AQ2" s="132"/>
       <c r="AR2" s="120"/>
       <c r="AS2" s="120"/>
-      <c r="AT2" s="121"/>
-      <c r="AU2" s="131"/>
-      <c r="AV2" s="132"/>
-      <c r="AW2" s="132"/>
-      <c r="AX2" s="132"/>
-      <c r="AY2" s="132"/>
-      <c r="AZ2" s="132"/>
-      <c r="BA2" s="133"/>
+      <c r="AT2" s="133"/>
+      <c r="AU2" s="153"/>
+      <c r="AV2" s="154"/>
+      <c r="AW2" s="154"/>
+      <c r="AX2" s="154"/>
+      <c r="AY2" s="154"/>
+      <c r="AZ2" s="154"/>
+      <c r="BA2" s="155"/>
       <c r="BC2" s="56"/>
       <c r="BD2" s="56"/>
       <c r="BE2" s="51"/>
@@ -6055,56 +6065,56 @@
     </row>
     <row r="3" spans="1:59" ht="12.6" customHeight="1">
       <c r="C3" s="53"/>
-      <c r="D3" s="156"/>
-      <c r="E3" s="157"/>
-      <c r="F3" s="126"/>
-      <c r="G3" s="142"/>
+      <c r="D3" s="149"/>
+      <c r="E3" s="150"/>
+      <c r="F3" s="142"/>
+      <c r="G3" s="132"/>
       <c r="H3" s="120"/>
       <c r="I3" s="120"/>
       <c r="J3" s="120"/>
       <c r="K3" s="120"/>
       <c r="L3" s="120"/>
       <c r="M3" s="120"/>
-      <c r="N3" s="121"/>
-      <c r="O3" s="152"/>
-      <c r="P3" s="153"/>
+      <c r="N3" s="133"/>
+      <c r="O3" s="145"/>
+      <c r="P3" s="146"/>
       <c r="Q3" s="160"/>
-      <c r="R3" s="125"/>
-      <c r="S3" s="126"/>
-      <c r="T3" s="145"/>
-      <c r="U3" s="148"/>
-      <c r="V3" s="149"/>
-      <c r="W3" s="125"/>
-      <c r="X3" s="126"/>
-      <c r="Y3" s="145"/>
-      <c r="Z3" s="148"/>
-      <c r="AA3" s="149"/>
-      <c r="AB3" s="152"/>
-      <c r="AC3" s="153"/>
-      <c r="AD3" s="125"/>
-      <c r="AE3" s="126"/>
-      <c r="AF3" s="140"/>
-      <c r="AG3" s="135"/>
-      <c r="AH3" s="135"/>
-      <c r="AI3" s="136"/>
-      <c r="AJ3" s="140"/>
-      <c r="AK3" s="135"/>
-      <c r="AL3" s="135"/>
-      <c r="AM3" s="136"/>
-      <c r="AN3" s="143"/>
-      <c r="AO3" s="143"/>
-      <c r="AP3" s="145"/>
-      <c r="AQ3" s="142"/>
+      <c r="R3" s="141"/>
+      <c r="S3" s="142"/>
+      <c r="T3" s="130"/>
+      <c r="U3" s="137"/>
+      <c r="V3" s="138"/>
+      <c r="W3" s="141"/>
+      <c r="X3" s="142"/>
+      <c r="Y3" s="130"/>
+      <c r="Z3" s="137"/>
+      <c r="AA3" s="138"/>
+      <c r="AB3" s="145"/>
+      <c r="AC3" s="146"/>
+      <c r="AD3" s="141"/>
+      <c r="AE3" s="142"/>
+      <c r="AF3" s="122"/>
+      <c r="AG3" s="123"/>
+      <c r="AH3" s="123"/>
+      <c r="AI3" s="124"/>
+      <c r="AJ3" s="122"/>
+      <c r="AK3" s="123"/>
+      <c r="AL3" s="123"/>
+      <c r="AM3" s="124"/>
+      <c r="AN3" s="128"/>
+      <c r="AO3" s="128"/>
+      <c r="AP3" s="130"/>
+      <c r="AQ3" s="132"/>
       <c r="AR3" s="120"/>
       <c r="AS3" s="120"/>
-      <c r="AT3" s="121"/>
-      <c r="AU3" s="131"/>
-      <c r="AV3" s="132"/>
-      <c r="AW3" s="132"/>
-      <c r="AX3" s="132"/>
-      <c r="AY3" s="132"/>
-      <c r="AZ3" s="132"/>
-      <c r="BA3" s="133"/>
+      <c r="AT3" s="133"/>
+      <c r="AU3" s="153"/>
+      <c r="AV3" s="154"/>
+      <c r="AW3" s="154"/>
+      <c r="AX3" s="154"/>
+      <c r="AY3" s="154"/>
+      <c r="AZ3" s="154"/>
+      <c r="BA3" s="155"/>
       <c r="BC3" s="50" t="s">
         <v>45</v>
       </c>
@@ -6118,56 +6128,56 @@
         <v>57</v>
       </c>
       <c r="C4" s="53"/>
-      <c r="D4" s="156"/>
-      <c r="E4" s="157"/>
-      <c r="F4" s="126"/>
-      <c r="G4" s="142"/>
+      <c r="D4" s="149"/>
+      <c r="E4" s="150"/>
+      <c r="F4" s="142"/>
+      <c r="G4" s="132"/>
       <c r="H4" s="120"/>
       <c r="I4" s="120"/>
       <c r="J4" s="120"/>
       <c r="K4" s="120"/>
       <c r="L4" s="120"/>
       <c r="M4" s="120"/>
-      <c r="N4" s="121"/>
-      <c r="O4" s="152"/>
-      <c r="P4" s="153"/>
+      <c r="N4" s="133"/>
+      <c r="O4" s="145"/>
+      <c r="P4" s="146"/>
       <c r="Q4" s="160"/>
-      <c r="R4" s="125"/>
-      <c r="S4" s="126"/>
-      <c r="T4" s="145"/>
-      <c r="U4" s="148"/>
-      <c r="V4" s="149"/>
-      <c r="W4" s="125"/>
-      <c r="X4" s="126"/>
-      <c r="Y4" s="145"/>
-      <c r="Z4" s="148"/>
-      <c r="AA4" s="149"/>
-      <c r="AB4" s="152"/>
-      <c r="AC4" s="153"/>
-      <c r="AD4" s="125"/>
-      <c r="AE4" s="126"/>
-      <c r="AF4" s="140"/>
-      <c r="AG4" s="135"/>
-      <c r="AH4" s="135"/>
-      <c r="AI4" s="136"/>
-      <c r="AJ4" s="140"/>
-      <c r="AK4" s="135"/>
-      <c r="AL4" s="135"/>
-      <c r="AM4" s="136"/>
-      <c r="AN4" s="143"/>
-      <c r="AO4" s="143"/>
-      <c r="AP4" s="145"/>
-      <c r="AQ4" s="142"/>
+      <c r="R4" s="141"/>
+      <c r="S4" s="142"/>
+      <c r="T4" s="130"/>
+      <c r="U4" s="137"/>
+      <c r="V4" s="138"/>
+      <c r="W4" s="141"/>
+      <c r="X4" s="142"/>
+      <c r="Y4" s="130"/>
+      <c r="Z4" s="137"/>
+      <c r="AA4" s="138"/>
+      <c r="AB4" s="145"/>
+      <c r="AC4" s="146"/>
+      <c r="AD4" s="141"/>
+      <c r="AE4" s="142"/>
+      <c r="AF4" s="122"/>
+      <c r="AG4" s="123"/>
+      <c r="AH4" s="123"/>
+      <c r="AI4" s="124"/>
+      <c r="AJ4" s="122"/>
+      <c r="AK4" s="123"/>
+      <c r="AL4" s="123"/>
+      <c r="AM4" s="124"/>
+      <c r="AN4" s="128"/>
+      <c r="AO4" s="128"/>
+      <c r="AP4" s="130"/>
+      <c r="AQ4" s="132"/>
       <c r="AR4" s="120"/>
       <c r="AS4" s="120"/>
-      <c r="AT4" s="121"/>
-      <c r="AU4" s="131"/>
-      <c r="AV4" s="132"/>
-      <c r="AW4" s="132"/>
-      <c r="AX4" s="132"/>
-      <c r="AY4" s="132"/>
-      <c r="AZ4" s="132"/>
-      <c r="BA4" s="133"/>
+      <c r="AT4" s="133"/>
+      <c r="AU4" s="153"/>
+      <c r="AV4" s="154"/>
+      <c r="AW4" s="154"/>
+      <c r="AX4" s="154"/>
+      <c r="AY4" s="154"/>
+      <c r="AZ4" s="154"/>
+      <c r="BA4" s="155"/>
       <c r="BC4" s="56"/>
       <c r="BD4" s="56"/>
     </row>
@@ -6175,56 +6185,56 @@
       <c r="C5" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="156"/>
-      <c r="E5" s="157"/>
-      <c r="F5" s="126"/>
-      <c r="G5" s="142"/>
+      <c r="D5" s="149"/>
+      <c r="E5" s="150"/>
+      <c r="F5" s="142"/>
+      <c r="G5" s="132"/>
       <c r="H5" s="120"/>
       <c r="I5" s="120"/>
       <c r="J5" s="120"/>
       <c r="K5" s="120"/>
       <c r="L5" s="120"/>
       <c r="M5" s="120"/>
-      <c r="N5" s="121"/>
-      <c r="O5" s="152"/>
-      <c r="P5" s="153"/>
+      <c r="N5" s="133"/>
+      <c r="O5" s="145"/>
+      <c r="P5" s="146"/>
       <c r="Q5" s="160"/>
-      <c r="R5" s="125"/>
-      <c r="S5" s="126"/>
-      <c r="T5" s="145"/>
-      <c r="U5" s="148"/>
-      <c r="V5" s="149"/>
-      <c r="W5" s="125"/>
-      <c r="X5" s="126"/>
-      <c r="Y5" s="145"/>
-      <c r="Z5" s="148"/>
-      <c r="AA5" s="149"/>
-      <c r="AB5" s="152"/>
-      <c r="AC5" s="153"/>
-      <c r="AD5" s="125"/>
-      <c r="AE5" s="126"/>
-      <c r="AF5" s="140"/>
-      <c r="AG5" s="135"/>
-      <c r="AH5" s="135"/>
-      <c r="AI5" s="136"/>
-      <c r="AJ5" s="140"/>
-      <c r="AK5" s="135"/>
-      <c r="AL5" s="135"/>
-      <c r="AM5" s="136"/>
-      <c r="AN5" s="143"/>
-      <c r="AO5" s="143"/>
-      <c r="AP5" s="145"/>
-      <c r="AQ5" s="142"/>
+      <c r="R5" s="141"/>
+      <c r="S5" s="142"/>
+      <c r="T5" s="130"/>
+      <c r="U5" s="137"/>
+      <c r="V5" s="138"/>
+      <c r="W5" s="141"/>
+      <c r="X5" s="142"/>
+      <c r="Y5" s="130"/>
+      <c r="Z5" s="137"/>
+      <c r="AA5" s="138"/>
+      <c r="AB5" s="145"/>
+      <c r="AC5" s="146"/>
+      <c r="AD5" s="141"/>
+      <c r="AE5" s="142"/>
+      <c r="AF5" s="122"/>
+      <c r="AG5" s="123"/>
+      <c r="AH5" s="123"/>
+      <c r="AI5" s="124"/>
+      <c r="AJ5" s="122"/>
+      <c r="AK5" s="123"/>
+      <c r="AL5" s="123"/>
+      <c r="AM5" s="124"/>
+      <c r="AN5" s="128"/>
+      <c r="AO5" s="128"/>
+      <c r="AP5" s="130"/>
+      <c r="AQ5" s="132"/>
       <c r="AR5" s="120"/>
       <c r="AS5" s="120"/>
-      <c r="AT5" s="121"/>
-      <c r="AU5" s="131"/>
-      <c r="AV5" s="132"/>
-      <c r="AW5" s="132"/>
-      <c r="AX5" s="132"/>
-      <c r="AY5" s="132"/>
-      <c r="AZ5" s="132"/>
-      <c r="BA5" s="133"/>
+      <c r="AT5" s="133"/>
+      <c r="AU5" s="153"/>
+      <c r="AV5" s="154"/>
+      <c r="AW5" s="154"/>
+      <c r="AX5" s="154"/>
+      <c r="AY5" s="154"/>
+      <c r="AZ5" s="154"/>
+      <c r="BA5" s="155"/>
       <c r="BC5" s="50" t="s">
         <v>47</v>
       </c>
@@ -6235,56 +6245,56 @@
         <v>58</v>
       </c>
       <c r="C6" s="53"/>
-      <c r="D6" s="158"/>
-      <c r="E6" s="159"/>
-      <c r="F6" s="128"/>
-      <c r="G6" s="147"/>
-      <c r="H6" s="123"/>
-      <c r="I6" s="123"/>
-      <c r="J6" s="123"/>
-      <c r="K6" s="123"/>
-      <c r="L6" s="123"/>
-      <c r="M6" s="123"/>
-      <c r="N6" s="124"/>
-      <c r="O6" s="154"/>
-      <c r="P6" s="155"/>
+      <c r="D6" s="151"/>
+      <c r="E6" s="152"/>
+      <c r="F6" s="144"/>
+      <c r="G6" s="134"/>
+      <c r="H6" s="135"/>
+      <c r="I6" s="135"/>
+      <c r="J6" s="135"/>
+      <c r="K6" s="135"/>
+      <c r="L6" s="135"/>
+      <c r="M6" s="135"/>
+      <c r="N6" s="136"/>
+      <c r="O6" s="147"/>
+      <c r="P6" s="148"/>
       <c r="Q6" s="161"/>
-      <c r="R6" s="127"/>
-      <c r="S6" s="128"/>
-      <c r="T6" s="146"/>
-      <c r="U6" s="150"/>
-      <c r="V6" s="151"/>
-      <c r="W6" s="127"/>
-      <c r="X6" s="128"/>
-      <c r="Y6" s="146"/>
-      <c r="Z6" s="150"/>
-      <c r="AA6" s="151"/>
-      <c r="AB6" s="154"/>
-      <c r="AC6" s="155"/>
-      <c r="AD6" s="127"/>
-      <c r="AE6" s="128"/>
-      <c r="AF6" s="141"/>
-      <c r="AG6" s="138"/>
-      <c r="AH6" s="138"/>
-      <c r="AI6" s="139"/>
-      <c r="AJ6" s="141"/>
-      <c r="AK6" s="138"/>
-      <c r="AL6" s="138"/>
-      <c r="AM6" s="139"/>
-      <c r="AN6" s="144"/>
-      <c r="AO6" s="144"/>
-      <c r="AP6" s="146"/>
-      <c r="AQ6" s="147"/>
-      <c r="AR6" s="123"/>
-      <c r="AS6" s="123"/>
-      <c r="AT6" s="124"/>
-      <c r="AU6" s="131"/>
-      <c r="AV6" s="132"/>
-      <c r="AW6" s="132"/>
-      <c r="AX6" s="132"/>
-      <c r="AY6" s="132"/>
-      <c r="AZ6" s="132"/>
-      <c r="BA6" s="133"/>
+      <c r="R6" s="143"/>
+      <c r="S6" s="144"/>
+      <c r="T6" s="131"/>
+      <c r="U6" s="139"/>
+      <c r="V6" s="140"/>
+      <c r="W6" s="143"/>
+      <c r="X6" s="144"/>
+      <c r="Y6" s="131"/>
+      <c r="Z6" s="139"/>
+      <c r="AA6" s="140"/>
+      <c r="AB6" s="147"/>
+      <c r="AC6" s="148"/>
+      <c r="AD6" s="143"/>
+      <c r="AE6" s="144"/>
+      <c r="AF6" s="125"/>
+      <c r="AG6" s="126"/>
+      <c r="AH6" s="126"/>
+      <c r="AI6" s="127"/>
+      <c r="AJ6" s="125"/>
+      <c r="AK6" s="126"/>
+      <c r="AL6" s="126"/>
+      <c r="AM6" s="127"/>
+      <c r="AN6" s="129"/>
+      <c r="AO6" s="129"/>
+      <c r="AP6" s="131"/>
+      <c r="AQ6" s="134"/>
+      <c r="AR6" s="135"/>
+      <c r="AS6" s="135"/>
+      <c r="AT6" s="136"/>
+      <c r="AU6" s="153"/>
+      <c r="AV6" s="154"/>
+      <c r="AW6" s="154"/>
+      <c r="AX6" s="154"/>
+      <c r="AY6" s="154"/>
+      <c r="AZ6" s="154"/>
+      <c r="BA6" s="155"/>
       <c r="BC6" s="56" t="s">
         <v>48</v>
       </c>
@@ -6604,23 +6614,23 @@
     </row>
     <row r="10" spans="1:59" ht="12.6" customHeight="1">
       <c r="C10" s="49"/>
-      <c r="D10" s="134" t="s">
+      <c r="D10" s="156" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="135"/>
-      <c r="F10" s="135"/>
-      <c r="G10" s="136"/>
-      <c r="H10" s="140" t="s">
+      <c r="E10" s="123"/>
+      <c r="F10" s="123"/>
+      <c r="G10" s="124"/>
+      <c r="H10" s="122" t="s">
         <v>42</v>
       </c>
-      <c r="I10" s="135"/>
-      <c r="J10" s="135"/>
-      <c r="K10" s="135"/>
-      <c r="L10" s="135"/>
-      <c r="M10" s="135"/>
-      <c r="N10" s="135"/>
-      <c r="O10" s="136"/>
-      <c r="P10" s="142" t="s">
+      <c r="I10" s="123"/>
+      <c r="J10" s="123"/>
+      <c r="K10" s="123"/>
+      <c r="L10" s="123"/>
+      <c r="M10" s="123"/>
+      <c r="N10" s="123"/>
+      <c r="O10" s="124"/>
+      <c r="P10" s="132" t="s">
         <v>148</v>
       </c>
       <c r="Q10" s="120"/>
@@ -6659,7 +6669,7 @@
       <c r="AX10" s="120"/>
       <c r="AY10" s="120"/>
       <c r="AZ10" s="120"/>
-      <c r="BA10" s="129"/>
+      <c r="BA10" s="121"/>
       <c r="BC10" s="56" t="s">
         <v>51</v>
       </c>
@@ -6669,19 +6679,19 @@
       <c r="C11" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="134"/>
-      <c r="E11" s="135"/>
-      <c r="F11" s="135"/>
-      <c r="G11" s="136"/>
-      <c r="H11" s="140"/>
-      <c r="I11" s="135"/>
-      <c r="J11" s="135"/>
-      <c r="K11" s="135"/>
-      <c r="L11" s="135"/>
-      <c r="M11" s="135"/>
-      <c r="N11" s="135"/>
-      <c r="O11" s="136"/>
-      <c r="P11" s="142"/>
+      <c r="D11" s="156"/>
+      <c r="E11" s="123"/>
+      <c r="F11" s="123"/>
+      <c r="G11" s="124"/>
+      <c r="H11" s="122"/>
+      <c r="I11" s="123"/>
+      <c r="J11" s="123"/>
+      <c r="K11" s="123"/>
+      <c r="L11" s="123"/>
+      <c r="M11" s="123"/>
+      <c r="N11" s="123"/>
+      <c r="O11" s="124"/>
+      <c r="P11" s="132"/>
       <c r="Q11" s="120"/>
       <c r="R11" s="120"/>
       <c r="S11" s="120"/>
@@ -6718,25 +6728,25 @@
       <c r="AX11" s="120"/>
       <c r="AY11" s="120"/>
       <c r="AZ11" s="120"/>
-      <c r="BA11" s="129"/>
+      <c r="BA11" s="121"/>
       <c r="BC11" s="106"/>
       <c r="BD11" s="106"/>
     </row>
     <row r="12" spans="1:59" ht="12.6" customHeight="1">
       <c r="C12" s="53"/>
-      <c r="D12" s="134"/>
-      <c r="E12" s="135"/>
-      <c r="F12" s="135"/>
-      <c r="G12" s="136"/>
-      <c r="H12" s="140"/>
-      <c r="I12" s="135"/>
-      <c r="J12" s="135"/>
-      <c r="K12" s="135"/>
-      <c r="L12" s="135"/>
-      <c r="M12" s="135"/>
-      <c r="N12" s="135"/>
-      <c r="O12" s="136"/>
-      <c r="P12" s="142"/>
+      <c r="D12" s="156"/>
+      <c r="E12" s="123"/>
+      <c r="F12" s="123"/>
+      <c r="G12" s="124"/>
+      <c r="H12" s="122"/>
+      <c r="I12" s="123"/>
+      <c r="J12" s="123"/>
+      <c r="K12" s="123"/>
+      <c r="L12" s="123"/>
+      <c r="M12" s="123"/>
+      <c r="N12" s="123"/>
+      <c r="O12" s="124"/>
+      <c r="P12" s="132"/>
       <c r="Q12" s="120"/>
       <c r="R12" s="120"/>
       <c r="S12" s="120"/>
@@ -6773,7 +6783,7 @@
       <c r="AX12" s="120"/>
       <c r="AY12" s="120"/>
       <c r="AZ12" s="120"/>
-      <c r="BA12" s="129"/>
+      <c r="BA12" s="121"/>
       <c r="BC12" s="56" t="s">
         <v>52</v>
       </c>
@@ -6786,19 +6796,19 @@
         <v>57</v>
       </c>
       <c r="C13" s="53"/>
-      <c r="D13" s="134"/>
-      <c r="E13" s="135"/>
-      <c r="F13" s="135"/>
-      <c r="G13" s="136"/>
-      <c r="H13" s="140"/>
-      <c r="I13" s="135"/>
-      <c r="J13" s="135"/>
-      <c r="K13" s="135"/>
-      <c r="L13" s="135"/>
-      <c r="M13" s="135"/>
-      <c r="N13" s="135"/>
-      <c r="O13" s="136"/>
-      <c r="P13" s="142"/>
+      <c r="D13" s="156"/>
+      <c r="E13" s="123"/>
+      <c r="F13" s="123"/>
+      <c r="G13" s="124"/>
+      <c r="H13" s="122"/>
+      <c r="I13" s="123"/>
+      <c r="J13" s="123"/>
+      <c r="K13" s="123"/>
+      <c r="L13" s="123"/>
+      <c r="M13" s="123"/>
+      <c r="N13" s="123"/>
+      <c r="O13" s="124"/>
+      <c r="P13" s="132"/>
       <c r="Q13" s="120"/>
       <c r="R13" s="120"/>
       <c r="S13" s="120"/>
@@ -6835,7 +6845,7 @@
       <c r="AX13" s="120"/>
       <c r="AY13" s="120"/>
       <c r="AZ13" s="120"/>
-      <c r="BA13" s="129"/>
+      <c r="BA13" s="121"/>
       <c r="BC13" s="56" t="s">
         <v>53</v>
       </c>
@@ -6845,19 +6855,19 @@
       <c r="C14" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="134"/>
-      <c r="E14" s="135"/>
-      <c r="F14" s="135"/>
-      <c r="G14" s="136"/>
-      <c r="H14" s="140"/>
-      <c r="I14" s="135"/>
-      <c r="J14" s="135"/>
-      <c r="K14" s="135"/>
-      <c r="L14" s="135"/>
-      <c r="M14" s="135"/>
-      <c r="N14" s="135"/>
-      <c r="O14" s="136"/>
-      <c r="P14" s="142"/>
+      <c r="D14" s="156"/>
+      <c r="E14" s="123"/>
+      <c r="F14" s="123"/>
+      <c r="G14" s="124"/>
+      <c r="H14" s="122"/>
+      <c r="I14" s="123"/>
+      <c r="J14" s="123"/>
+      <c r="K14" s="123"/>
+      <c r="L14" s="123"/>
+      <c r="M14" s="123"/>
+      <c r="N14" s="123"/>
+      <c r="O14" s="124"/>
+      <c r="P14" s="132"/>
       <c r="Q14" s="120"/>
       <c r="R14" s="120"/>
       <c r="S14" s="120"/>
@@ -6894,7 +6904,7 @@
       <c r="AX14" s="120"/>
       <c r="AY14" s="120"/>
       <c r="AZ14" s="120"/>
-      <c r="BA14" s="129"/>
+      <c r="BA14" s="121"/>
       <c r="BC14" s="50" t="s">
         <v>54</v>
       </c>
@@ -6905,19 +6915,19 @@
         <v>59</v>
       </c>
       <c r="C15" s="53"/>
-      <c r="D15" s="137"/>
-      <c r="E15" s="138"/>
-      <c r="F15" s="138"/>
-      <c r="G15" s="139"/>
-      <c r="H15" s="141"/>
-      <c r="I15" s="138"/>
-      <c r="J15" s="138"/>
-      <c r="K15" s="138"/>
-      <c r="L15" s="138"/>
-      <c r="M15" s="138"/>
-      <c r="N15" s="138"/>
-      <c r="O15" s="139"/>
-      <c r="P15" s="142"/>
+      <c r="D15" s="157"/>
+      <c r="E15" s="126"/>
+      <c r="F15" s="126"/>
+      <c r="G15" s="127"/>
+      <c r="H15" s="125"/>
+      <c r="I15" s="126"/>
+      <c r="J15" s="126"/>
+      <c r="K15" s="126"/>
+      <c r="L15" s="126"/>
+      <c r="M15" s="126"/>
+      <c r="N15" s="126"/>
+      <c r="O15" s="127"/>
+      <c r="P15" s="132"/>
       <c r="Q15" s="120"/>
       <c r="R15" s="120"/>
       <c r="S15" s="120"/>
@@ -6954,7 +6964,7 @@
       <c r="AX15" s="120"/>
       <c r="AY15" s="120"/>
       <c r="AZ15" s="120"/>
-      <c r="BA15" s="129"/>
+      <c r="BA15" s="121"/>
       <c r="BC15" s="56" t="s">
         <v>53</v>
       </c>
@@ -7296,7 +7306,7 @@
       <c r="AX19" s="120"/>
       <c r="AY19" s="120"/>
       <c r="AZ19" s="120"/>
-      <c r="BA19" s="129"/>
+      <c r="BA19" s="121"/>
       <c r="BC19" s="107" t="s">
         <v>56</v>
       </c>
@@ -7355,7 +7365,7 @@
       <c r="AX20" s="120"/>
       <c r="AY20" s="120"/>
       <c r="AZ20" s="120"/>
-      <c r="BA20" s="129"/>
+      <c r="BA20" s="121"/>
       <c r="BC20" s="64"/>
       <c r="BD20" s="62"/>
     </row>
@@ -7410,7 +7420,7 @@
       <c r="AX21" s="120"/>
       <c r="AY21" s="120"/>
       <c r="AZ21" s="120"/>
-      <c r="BA21" s="129"/>
+      <c r="BA21" s="121"/>
       <c r="BC21" s="64"/>
       <c r="BD21" s="62"/>
     </row>
@@ -7468,7 +7478,7 @@
       <c r="AX22" s="120"/>
       <c r="AY22" s="120"/>
       <c r="AZ22" s="120"/>
-      <c r="BA22" s="129"/>
+      <c r="BA22" s="121"/>
       <c r="BC22" s="64"/>
       <c r="BD22" s="62"/>
     </row>
@@ -7525,7 +7535,7 @@
       <c r="AX23" s="120"/>
       <c r="AY23" s="120"/>
       <c r="AZ23" s="120"/>
-      <c r="BA23" s="129"/>
+      <c r="BA23" s="121"/>
       <c r="BC23" s="64"/>
       <c r="BD23" s="62"/>
     </row>
@@ -7534,56 +7544,56 @@
         <v>61</v>
       </c>
       <c r="C24" s="53"/>
-      <c r="D24" s="122"/>
-      <c r="E24" s="123"/>
-      <c r="F24" s="123"/>
-      <c r="G24" s="123"/>
-      <c r="H24" s="123"/>
-      <c r="I24" s="123"/>
-      <c r="J24" s="123"/>
-      <c r="K24" s="123"/>
-      <c r="L24" s="123"/>
-      <c r="M24" s="123"/>
-      <c r="N24" s="123"/>
-      <c r="O24" s="123"/>
-      <c r="P24" s="123"/>
-      <c r="Q24" s="123"/>
-      <c r="R24" s="123"/>
-      <c r="S24" s="123"/>
-      <c r="T24" s="123"/>
-      <c r="U24" s="123"/>
-      <c r="V24" s="123"/>
-      <c r="W24" s="123"/>
-      <c r="X24" s="123"/>
-      <c r="Y24" s="123"/>
-      <c r="Z24" s="123"/>
-      <c r="AA24" s="123"/>
-      <c r="AB24" s="123"/>
-      <c r="AC24" s="123"/>
-      <c r="AD24" s="123"/>
-      <c r="AE24" s="123"/>
-      <c r="AF24" s="123"/>
-      <c r="AG24" s="123"/>
-      <c r="AH24" s="123"/>
-      <c r="AI24" s="123"/>
-      <c r="AJ24" s="123"/>
-      <c r="AK24" s="123"/>
-      <c r="AL24" s="123"/>
-      <c r="AM24" s="123"/>
-      <c r="AN24" s="123"/>
-      <c r="AO24" s="123"/>
-      <c r="AP24" s="123"/>
-      <c r="AQ24" s="123"/>
-      <c r="AR24" s="123"/>
-      <c r="AS24" s="123"/>
-      <c r="AT24" s="123"/>
-      <c r="AU24" s="123"/>
-      <c r="AV24" s="123"/>
-      <c r="AW24" s="123"/>
-      <c r="AX24" s="123"/>
-      <c r="AY24" s="123"/>
-      <c r="AZ24" s="123"/>
-      <c r="BA24" s="130"/>
+      <c r="D24" s="158"/>
+      <c r="E24" s="135"/>
+      <c r="F24" s="135"/>
+      <c r="G24" s="135"/>
+      <c r="H24" s="135"/>
+      <c r="I24" s="135"/>
+      <c r="J24" s="135"/>
+      <c r="K24" s="135"/>
+      <c r="L24" s="135"/>
+      <c r="M24" s="135"/>
+      <c r="N24" s="135"/>
+      <c r="O24" s="135"/>
+      <c r="P24" s="135"/>
+      <c r="Q24" s="135"/>
+      <c r="R24" s="135"/>
+      <c r="S24" s="135"/>
+      <c r="T24" s="135"/>
+      <c r="U24" s="135"/>
+      <c r="V24" s="135"/>
+      <c r="W24" s="135"/>
+      <c r="X24" s="135"/>
+      <c r="Y24" s="135"/>
+      <c r="Z24" s="135"/>
+      <c r="AA24" s="135"/>
+      <c r="AB24" s="135"/>
+      <c r="AC24" s="135"/>
+      <c r="AD24" s="135"/>
+      <c r="AE24" s="135"/>
+      <c r="AF24" s="135"/>
+      <c r="AG24" s="135"/>
+      <c r="AH24" s="135"/>
+      <c r="AI24" s="135"/>
+      <c r="AJ24" s="135"/>
+      <c r="AK24" s="135"/>
+      <c r="AL24" s="135"/>
+      <c r="AM24" s="135"/>
+      <c r="AN24" s="135"/>
+      <c r="AO24" s="135"/>
+      <c r="AP24" s="135"/>
+      <c r="AQ24" s="135"/>
+      <c r="AR24" s="135"/>
+      <c r="AS24" s="135"/>
+      <c r="AT24" s="135"/>
+      <c r="AU24" s="135"/>
+      <c r="AV24" s="135"/>
+      <c r="AW24" s="135"/>
+      <c r="AX24" s="135"/>
+      <c r="AY24" s="135"/>
+      <c r="AZ24" s="135"/>
+      <c r="BA24" s="159"/>
       <c r="BC24" s="64"/>
       <c r="BD24" s="62"/>
     </row>
@@ -7918,7 +7928,7 @@
       <c r="AX28" s="120"/>
       <c r="AY28" s="120"/>
       <c r="AZ28" s="120"/>
-      <c r="BA28" s="129"/>
+      <c r="BA28" s="121"/>
       <c r="BC28" s="64"/>
       <c r="BD28" s="62"/>
     </row>
@@ -7975,7 +7985,7 @@
       <c r="AX29" s="120"/>
       <c r="AY29" s="120"/>
       <c r="AZ29" s="120"/>
-      <c r="BA29" s="129"/>
+      <c r="BA29" s="121"/>
       <c r="BC29" s="64"/>
       <c r="BD29" s="62"/>
     </row>
@@ -8030,7 +8040,7 @@
       <c r="AX30" s="120"/>
       <c r="AY30" s="120"/>
       <c r="AZ30" s="120"/>
-      <c r="BA30" s="129"/>
+      <c r="BA30" s="121"/>
       <c r="BC30" s="64"/>
       <c r="BD30" s="62"/>
     </row>
@@ -8088,7 +8098,7 @@
       <c r="AX31" s="120"/>
       <c r="AY31" s="120"/>
       <c r="AZ31" s="120"/>
-      <c r="BA31" s="129"/>
+      <c r="BA31" s="121"/>
       <c r="BC31" s="64"/>
       <c r="BD31" s="62"/>
     </row>
@@ -8145,7 +8155,7 @@
       <c r="AX32" s="120"/>
       <c r="AY32" s="120"/>
       <c r="AZ32" s="120"/>
-      <c r="BA32" s="129"/>
+      <c r="BA32" s="121"/>
       <c r="BC32" s="64"/>
       <c r="BD32" s="62"/>
     </row>
@@ -8203,7 +8213,7 @@
       <c r="AX33" s="120"/>
       <c r="AY33" s="120"/>
       <c r="AZ33" s="120"/>
-      <c r="BA33" s="129"/>
+      <c r="BA33" s="121"/>
       <c r="BC33" s="64"/>
       <c r="BD33" s="62"/>
     </row>
@@ -8537,7 +8547,7 @@
       <c r="AX37" s="120"/>
       <c r="AY37" s="120"/>
       <c r="AZ37" s="120"/>
-      <c r="BA37" s="129"/>
+      <c r="BA37" s="121"/>
       <c r="BC37" s="64"/>
       <c r="BD37" s="62"/>
     </row>
@@ -8594,7 +8604,7 @@
       <c r="AX38" s="120"/>
       <c r="AY38" s="120"/>
       <c r="AZ38" s="120"/>
-      <c r="BA38" s="129"/>
+      <c r="BA38" s="121"/>
       <c r="BC38" s="64"/>
       <c r="BD38" s="62"/>
     </row>
@@ -8649,7 +8659,7 @@
       <c r="AX39" s="120"/>
       <c r="AY39" s="120"/>
       <c r="AZ39" s="120"/>
-      <c r="BA39" s="129"/>
+      <c r="BA39" s="121"/>
       <c r="BC39" s="64"/>
       <c r="BD39" s="62"/>
     </row>
@@ -8707,7 +8717,7 @@
       <c r="AX40" s="120"/>
       <c r="AY40" s="120"/>
       <c r="AZ40" s="120"/>
-      <c r="BA40" s="129"/>
+      <c r="BA40" s="121"/>
       <c r="BC40" s="64"/>
       <c r="BD40" s="62"/>
     </row>
@@ -8764,7 +8774,7 @@
       <c r="AX41" s="120"/>
       <c r="AY41" s="120"/>
       <c r="AZ41" s="120"/>
-      <c r="BA41" s="129"/>
+      <c r="BA41" s="121"/>
       <c r="BC41" s="64"/>
       <c r="BD41" s="62"/>
     </row>
@@ -8773,56 +8783,56 @@
         <v>63</v>
       </c>
       <c r="C42" s="53"/>
-      <c r="D42" s="122"/>
-      <c r="E42" s="123"/>
-      <c r="F42" s="123"/>
-      <c r="G42" s="123"/>
-      <c r="H42" s="123"/>
-      <c r="I42" s="123"/>
-      <c r="J42" s="123"/>
-      <c r="K42" s="123"/>
-      <c r="L42" s="123"/>
-      <c r="M42" s="123"/>
-      <c r="N42" s="123"/>
-      <c r="O42" s="123"/>
-      <c r="P42" s="123"/>
-      <c r="Q42" s="123"/>
-      <c r="R42" s="123"/>
-      <c r="S42" s="123"/>
-      <c r="T42" s="123"/>
-      <c r="U42" s="123"/>
-      <c r="V42" s="123"/>
-      <c r="W42" s="123"/>
-      <c r="X42" s="123"/>
-      <c r="Y42" s="123"/>
-      <c r="Z42" s="123"/>
-      <c r="AA42" s="123"/>
-      <c r="AB42" s="123"/>
-      <c r="AC42" s="123"/>
-      <c r="AD42" s="123"/>
-      <c r="AE42" s="123"/>
-      <c r="AF42" s="123"/>
-      <c r="AG42" s="123"/>
-      <c r="AH42" s="123"/>
-      <c r="AI42" s="123"/>
-      <c r="AJ42" s="123"/>
-      <c r="AK42" s="123"/>
-      <c r="AL42" s="123"/>
-      <c r="AM42" s="123"/>
-      <c r="AN42" s="123"/>
-      <c r="AO42" s="123"/>
-      <c r="AP42" s="123"/>
-      <c r="AQ42" s="123"/>
-      <c r="AR42" s="123"/>
-      <c r="AS42" s="123"/>
-      <c r="AT42" s="123"/>
-      <c r="AU42" s="123"/>
-      <c r="AV42" s="123"/>
-      <c r="AW42" s="123"/>
-      <c r="AX42" s="123"/>
-      <c r="AY42" s="123"/>
-      <c r="AZ42" s="123"/>
-      <c r="BA42" s="130"/>
+      <c r="D42" s="158"/>
+      <c r="E42" s="135"/>
+      <c r="F42" s="135"/>
+      <c r="G42" s="135"/>
+      <c r="H42" s="135"/>
+      <c r="I42" s="135"/>
+      <c r="J42" s="135"/>
+      <c r="K42" s="135"/>
+      <c r="L42" s="135"/>
+      <c r="M42" s="135"/>
+      <c r="N42" s="135"/>
+      <c r="O42" s="135"/>
+      <c r="P42" s="135"/>
+      <c r="Q42" s="135"/>
+      <c r="R42" s="135"/>
+      <c r="S42" s="135"/>
+      <c r="T42" s="135"/>
+      <c r="U42" s="135"/>
+      <c r="V42" s="135"/>
+      <c r="W42" s="135"/>
+      <c r="X42" s="135"/>
+      <c r="Y42" s="135"/>
+      <c r="Z42" s="135"/>
+      <c r="AA42" s="135"/>
+      <c r="AB42" s="135"/>
+      <c r="AC42" s="135"/>
+      <c r="AD42" s="135"/>
+      <c r="AE42" s="135"/>
+      <c r="AF42" s="135"/>
+      <c r="AG42" s="135"/>
+      <c r="AH42" s="135"/>
+      <c r="AI42" s="135"/>
+      <c r="AJ42" s="135"/>
+      <c r="AK42" s="135"/>
+      <c r="AL42" s="135"/>
+      <c r="AM42" s="135"/>
+      <c r="AN42" s="135"/>
+      <c r="AO42" s="135"/>
+      <c r="AP42" s="135"/>
+      <c r="AQ42" s="135"/>
+      <c r="AR42" s="135"/>
+      <c r="AS42" s="135"/>
+      <c r="AT42" s="135"/>
+      <c r="AU42" s="135"/>
+      <c r="AV42" s="135"/>
+      <c r="AW42" s="135"/>
+      <c r="AX42" s="135"/>
+      <c r="AY42" s="135"/>
+      <c r="AZ42" s="135"/>
+      <c r="BA42" s="159"/>
       <c r="BC42" s="64"/>
       <c r="BD42" s="62"/>
     </row>
@@ -9158,7 +9168,7 @@
       <c r="AX46" s="120"/>
       <c r="AY46" s="120"/>
       <c r="AZ46" s="120"/>
-      <c r="BA46" s="129"/>
+      <c r="BA46" s="121"/>
       <c r="BC46" s="109" t="s">
         <v>47</v>
       </c>
@@ -9217,7 +9227,7 @@
       <c r="AX47" s="120"/>
       <c r="AY47" s="120"/>
       <c r="AZ47" s="120"/>
-      <c r="BA47" s="129"/>
+      <c r="BA47" s="121"/>
       <c r="BC47" s="64"/>
       <c r="BD47" s="62"/>
     </row>
@@ -9272,7 +9282,7 @@
       <c r="AX48" s="120"/>
       <c r="AY48" s="120"/>
       <c r="AZ48" s="120"/>
-      <c r="BA48" s="129"/>
+      <c r="BA48" s="121"/>
       <c r="BC48" s="64"/>
       <c r="BD48" s="62"/>
     </row>
@@ -9330,7 +9340,7 @@
       <c r="AX49" s="120"/>
       <c r="AY49" s="120"/>
       <c r="AZ49" s="120"/>
-      <c r="BA49" s="129"/>
+      <c r="BA49" s="121"/>
       <c r="BC49" s="64"/>
       <c r="BD49" s="62"/>
     </row>
@@ -9387,7 +9397,7 @@
       <c r="AX50" s="120"/>
       <c r="AY50" s="120"/>
       <c r="AZ50" s="120"/>
-      <c r="BA50" s="129"/>
+      <c r="BA50" s="121"/>
       <c r="BC50" s="64"/>
       <c r="BD50" s="62"/>
     </row>
@@ -9445,7 +9455,7 @@
       <c r="AX51" s="120"/>
       <c r="AY51" s="120"/>
       <c r="AZ51" s="120"/>
-      <c r="BA51" s="129"/>
+      <c r="BA51" s="121"/>
       <c r="BC51" s="64"/>
       <c r="BD51" s="62"/>
     </row>
@@ -9779,7 +9789,7 @@
       <c r="AX55" s="120"/>
       <c r="AY55" s="120"/>
       <c r="AZ55" s="120"/>
-      <c r="BA55" s="129"/>
+      <c r="BA55" s="121"/>
       <c r="BC55" s="64"/>
       <c r="BD55" s="62"/>
     </row>
@@ -9836,7 +9846,7 @@
       <c r="AX56" s="120"/>
       <c r="AY56" s="120"/>
       <c r="AZ56" s="120"/>
-      <c r="BA56" s="129"/>
+      <c r="BA56" s="121"/>
       <c r="BC56" s="64"/>
       <c r="BD56" s="62"/>
     </row>
@@ -9891,7 +9901,7 @@
       <c r="AX57" s="120"/>
       <c r="AY57" s="120"/>
       <c r="AZ57" s="120"/>
-      <c r="BA57" s="129"/>
+      <c r="BA57" s="121"/>
       <c r="BC57" s="64"/>
       <c r="BD57" s="62"/>
     </row>
@@ -9949,7 +9959,7 @@
       <c r="AX58" s="120"/>
       <c r="AY58" s="120"/>
       <c r="AZ58" s="120"/>
-      <c r="BA58" s="129"/>
+      <c r="BA58" s="121"/>
       <c r="BC58" s="64"/>
       <c r="BD58" s="62"/>
     </row>
@@ -10006,7 +10016,7 @@
       <c r="AX59" s="120"/>
       <c r="AY59" s="120"/>
       <c r="AZ59" s="120"/>
-      <c r="BA59" s="129"/>
+      <c r="BA59" s="121"/>
       <c r="BC59" s="64"/>
       <c r="BD59" s="62"/>
     </row>
@@ -10064,7 +10074,7 @@
       <c r="AX60" s="120"/>
       <c r="AY60" s="120"/>
       <c r="AZ60" s="120"/>
-      <c r="BA60" s="129"/>
+      <c r="BA60" s="121"/>
       <c r="BC60" s="64"/>
       <c r="BD60" s="62"/>
     </row>
@@ -10399,7 +10409,7 @@
       <c r="AX64" s="120"/>
       <c r="AY64" s="120"/>
       <c r="AZ64" s="120"/>
-      <c r="BA64" s="129"/>
+      <c r="BA64" s="121"/>
       <c r="BC64" s="64"/>
       <c r="BD64" s="62"/>
     </row>
@@ -10456,7 +10466,7 @@
       <c r="AX65" s="120"/>
       <c r="AY65" s="120"/>
       <c r="AZ65" s="120"/>
-      <c r="BA65" s="129"/>
+      <c r="BA65" s="121"/>
       <c r="BC65" s="64"/>
       <c r="BD65" s="62"/>
     </row>
@@ -10511,7 +10521,7 @@
       <c r="AX66" s="120"/>
       <c r="AY66" s="120"/>
       <c r="AZ66" s="120"/>
-      <c r="BA66" s="129"/>
+      <c r="BA66" s="121"/>
       <c r="BC66" s="64"/>
       <c r="BD66" s="62"/>
     </row>
@@ -10569,7 +10579,7 @@
       <c r="AX67" s="120"/>
       <c r="AY67" s="120"/>
       <c r="AZ67" s="120"/>
-      <c r="BA67" s="129"/>
+      <c r="BA67" s="121"/>
       <c r="BC67" s="64"/>
       <c r="BD67" s="62"/>
     </row>
@@ -10626,7 +10636,7 @@
       <c r="AX68" s="120"/>
       <c r="AY68" s="120"/>
       <c r="AZ68" s="120"/>
-      <c r="BA68" s="129"/>
+      <c r="BA68" s="121"/>
       <c r="BC68" s="64"/>
       <c r="BD68" s="62"/>
     </row>
@@ -10684,7 +10694,7 @@
       <c r="AX69" s="120"/>
       <c r="AY69" s="120"/>
       <c r="AZ69" s="120"/>
-      <c r="BA69" s="129"/>
+      <c r="BA69" s="121"/>
       <c r="BC69" s="64"/>
       <c r="BD69" s="62"/>
     </row>
@@ -11018,7 +11028,7 @@
       <c r="AX73" s="120"/>
       <c r="AY73" s="120"/>
       <c r="AZ73" s="120"/>
-      <c r="BA73" s="129"/>
+      <c r="BA73" s="121"/>
       <c r="BC73" s="64"/>
       <c r="BD73" s="62"/>
     </row>
@@ -11075,7 +11085,7 @@
       <c r="AX74" s="120"/>
       <c r="AY74" s="120"/>
       <c r="AZ74" s="120"/>
-      <c r="BA74" s="129"/>
+      <c r="BA74" s="121"/>
       <c r="BC74" s="64"/>
       <c r="BD74" s="62"/>
     </row>
@@ -11130,7 +11140,7 @@
       <c r="AX75" s="120"/>
       <c r="AY75" s="120"/>
       <c r="AZ75" s="120"/>
-      <c r="BA75" s="129"/>
+      <c r="BA75" s="121"/>
       <c r="BC75" s="64"/>
       <c r="BD75" s="62"/>
     </row>
@@ -11188,7 +11198,7 @@
       <c r="AX76" s="120"/>
       <c r="AY76" s="120"/>
       <c r="AZ76" s="120"/>
-      <c r="BA76" s="129"/>
+      <c r="BA76" s="121"/>
       <c r="BC76" s="64"/>
       <c r="BD76" s="62"/>
     </row>
@@ -11245,7 +11255,7 @@
       <c r="AX77" s="120"/>
       <c r="AY77" s="120"/>
       <c r="AZ77" s="120"/>
-      <c r="BA77" s="129"/>
+      <c r="BA77" s="121"/>
       <c r="BC77" s="64"/>
       <c r="BD77" s="62"/>
     </row>
@@ -11303,7 +11313,7 @@
       <c r="AX78" s="120"/>
       <c r="AY78" s="120"/>
       <c r="AZ78" s="120"/>
-      <c r="BA78" s="129"/>
+      <c r="BA78" s="121"/>
       <c r="BC78" s="64"/>
       <c r="BD78" s="62"/>
     </row>
@@ -11638,7 +11648,7 @@
       <c r="AX82" s="120"/>
       <c r="AY82" s="120"/>
       <c r="AZ82" s="120"/>
-      <c r="BA82" s="129"/>
+      <c r="BA82" s="121"/>
       <c r="BC82" s="64"/>
       <c r="BD82" s="62"/>
     </row>
@@ -11695,7 +11705,7 @@
       <c r="AX83" s="120"/>
       <c r="AY83" s="120"/>
       <c r="AZ83" s="120"/>
-      <c r="BA83" s="129"/>
+      <c r="BA83" s="121"/>
       <c r="BC83" s="64"/>
       <c r="BD83" s="62"/>
     </row>
@@ -11750,7 +11760,7 @@
       <c r="AX84" s="120"/>
       <c r="AY84" s="120"/>
       <c r="AZ84" s="120"/>
-      <c r="BA84" s="129"/>
+      <c r="BA84" s="121"/>
       <c r="BC84" s="64"/>
       <c r="BD84" s="62"/>
     </row>
@@ -11808,7 +11818,7 @@
       <c r="AX85" s="120"/>
       <c r="AY85" s="120"/>
       <c r="AZ85" s="120"/>
-      <c r="BA85" s="129"/>
+      <c r="BA85" s="121"/>
       <c r="BC85" s="64"/>
       <c r="BD85" s="62"/>
     </row>
@@ -11865,7 +11875,7 @@
       <c r="AX86" s="120"/>
       <c r="AY86" s="120"/>
       <c r="AZ86" s="120"/>
-      <c r="BA86" s="129"/>
+      <c r="BA86" s="121"/>
       <c r="BC86" s="64"/>
       <c r="BD86" s="62"/>
     </row>
@@ -11923,7 +11933,7 @@
       <c r="AX87" s="120"/>
       <c r="AY87" s="120"/>
       <c r="AZ87" s="120"/>
-      <c r="BA87" s="129"/>
+      <c r="BA87" s="121"/>
       <c r="BC87" s="64"/>
       <c r="BD87" s="62"/>
     </row>
@@ -12217,11 +12227,11 @@
       <c r="J91" s="120"/>
       <c r="K91" s="120"/>
       <c r="L91" s="120"/>
-      <c r="M91" s="121"/>
-      <c r="N91" s="125" t="s">
+      <c r="M91" s="133"/>
+      <c r="N91" s="141" t="s">
         <v>43</v>
       </c>
-      <c r="O91" s="126"/>
+      <c r="O91" s="142"/>
       <c r="P91" s="95"/>
       <c r="Q91" s="95"/>
       <c r="R91" s="95"/>
@@ -12278,9 +12288,9 @@
       <c r="J92" s="120"/>
       <c r="K92" s="120"/>
       <c r="L92" s="120"/>
-      <c r="M92" s="121"/>
-      <c r="N92" s="125"/>
-      <c r="O92" s="126"/>
+      <c r="M92" s="133"/>
+      <c r="N92" s="141"/>
+      <c r="O92" s="142"/>
       <c r="BA92" s="55"/>
       <c r="BC92" s="64"/>
       <c r="BD92" s="62"/>
@@ -12296,9 +12306,9 @@
       <c r="J93" s="120"/>
       <c r="K93" s="120"/>
       <c r="L93" s="120"/>
-      <c r="M93" s="121"/>
-      <c r="N93" s="125"/>
-      <c r="O93" s="126"/>
+      <c r="M93" s="133"/>
+      <c r="N93" s="141"/>
+      <c r="O93" s="142"/>
       <c r="BA93" s="55"/>
       <c r="BC93" s="64"/>
       <c r="BD93" s="62"/>
@@ -12317,9 +12327,9 @@
       <c r="J94" s="120"/>
       <c r="K94" s="120"/>
       <c r="L94" s="120"/>
-      <c r="M94" s="121"/>
-      <c r="N94" s="125"/>
-      <c r="O94" s="126"/>
+      <c r="M94" s="133"/>
+      <c r="N94" s="141"/>
+      <c r="O94" s="142"/>
       <c r="BA94" s="55"/>
       <c r="BC94" s="64"/>
       <c r="BD94" s="62"/>
@@ -12337,9 +12347,9 @@
       <c r="J95" s="120"/>
       <c r="K95" s="120"/>
       <c r="L95" s="120"/>
-      <c r="M95" s="121"/>
-      <c r="N95" s="125"/>
-      <c r="O95" s="126"/>
+      <c r="M95" s="133"/>
+      <c r="N95" s="141"/>
+      <c r="O95" s="142"/>
       <c r="BA95" s="55"/>
       <c r="BC95" s="64"/>
       <c r="BD95" s="62"/>
@@ -12349,18 +12359,18 @@
         <v>69</v>
       </c>
       <c r="C96" s="53"/>
-      <c r="D96" s="122"/>
-      <c r="E96" s="123"/>
-      <c r="F96" s="123"/>
-      <c r="G96" s="123"/>
-      <c r="H96" s="123"/>
-      <c r="I96" s="123"/>
-      <c r="J96" s="123"/>
-      <c r="K96" s="123"/>
-      <c r="L96" s="123"/>
-      <c r="M96" s="124"/>
-      <c r="N96" s="127"/>
-      <c r="O96" s="128"/>
+      <c r="D96" s="158"/>
+      <c r="E96" s="135"/>
+      <c r="F96" s="135"/>
+      <c r="G96" s="135"/>
+      <c r="H96" s="135"/>
+      <c r="I96" s="135"/>
+      <c r="J96" s="135"/>
+      <c r="K96" s="135"/>
+      <c r="L96" s="135"/>
+      <c r="M96" s="136"/>
+      <c r="N96" s="143"/>
+      <c r="O96" s="144"/>
       <c r="P96" s="97"/>
       <c r="Q96" s="97"/>
       <c r="R96" s="97"/>
@@ -14373,6 +14383,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="D91:M96"/>
+    <mergeCell ref="N91:O96"/>
+    <mergeCell ref="D37:BA42"/>
+    <mergeCell ref="D46:BA51"/>
+    <mergeCell ref="D55:BA60"/>
+    <mergeCell ref="D64:BA69"/>
+    <mergeCell ref="D73:BA78"/>
+    <mergeCell ref="D82:BA87"/>
+    <mergeCell ref="AU1:BA6"/>
+    <mergeCell ref="D10:G15"/>
+    <mergeCell ref="H10:O15"/>
+    <mergeCell ref="P10:BA15"/>
+    <mergeCell ref="D19:BA24"/>
+    <mergeCell ref="Q1:Q6"/>
+    <mergeCell ref="R1:S6"/>
+    <mergeCell ref="T1:T6"/>
     <mergeCell ref="D28:BA33"/>
     <mergeCell ref="AF1:AI6"/>
     <mergeCell ref="AJ1:AM6"/>
@@ -14389,22 +14415,6 @@
     <mergeCell ref="D1:F6"/>
     <mergeCell ref="G1:N6"/>
     <mergeCell ref="O1:P6"/>
-    <mergeCell ref="AU1:BA6"/>
-    <mergeCell ref="D10:G15"/>
-    <mergeCell ref="H10:O15"/>
-    <mergeCell ref="P10:BA15"/>
-    <mergeCell ref="D19:BA24"/>
-    <mergeCell ref="Q1:Q6"/>
-    <mergeCell ref="R1:S6"/>
-    <mergeCell ref="T1:T6"/>
-    <mergeCell ref="D91:M96"/>
-    <mergeCell ref="N91:O96"/>
-    <mergeCell ref="D37:BA42"/>
-    <mergeCell ref="D46:BA51"/>
-    <mergeCell ref="D55:BA60"/>
-    <mergeCell ref="D64:BA69"/>
-    <mergeCell ref="D73:BA78"/>
-    <mergeCell ref="D82:BA87"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <printOptions horizontalCentered="1" gridLinesSet="0"/>

</xml_diff>